<commit_message>
No Changes, excel file flipping a bitch
</commit_message>
<xml_diff>
--- a/project timeline.xlsx
+++ b/project timeline.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7680"/>
+    <workbookView xWindow="700" yWindow="100" windowWidth="25320" windowHeight="15160"/>
   </bookViews>
   <sheets>
     <sheet name="Project Timeline" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,12 @@
     <definedName name="WindowDays">calcs!$D$29</definedName>
     <definedName name="WindowOffset">calcs!$D$26</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -483,10 +488,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0"/>
-          <c:y val="0"/>
-          <c:w val="1"/>
-          <c:h val="1"/>
+          <c:x val="0.0"/>
+          <c:y val="0.0"/>
+          <c:w val="1.0"/>
+          <c:h val="1.0"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -535,97 +540,97 @@
             <c:numRef>
               <c:f>calcs!$E$31:$AH$31</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>41932</c:v>
+                  <c:v>41932.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41933</c:v>
+                  <c:v>41933.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41934</c:v>
+                  <c:v>41934.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41935</c:v>
+                  <c:v>41935.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41936</c:v>
+                  <c:v>41936.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>41937</c:v>
+                  <c:v>41937.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>41938</c:v>
+                  <c:v>41938.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>41939</c:v>
+                  <c:v>41939.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>41940</c:v>
+                  <c:v>41940.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>41941</c:v>
+                  <c:v>41941.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>41942</c:v>
+                  <c:v>41942.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>41943</c:v>
+                  <c:v>41943.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>41944</c:v>
+                  <c:v>41944.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>41945</c:v>
+                  <c:v>41945.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>41946</c:v>
+                  <c:v>41946.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>41947</c:v>
+                  <c:v>41947.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>41948</c:v>
+                  <c:v>41948.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>41949</c:v>
+                  <c:v>41949.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>41950</c:v>
+                  <c:v>41950.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>41951</c:v>
+                  <c:v>41951.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>41952</c:v>
+                  <c:v>41952.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>41953</c:v>
+                  <c:v>41953.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>41954</c:v>
+                  <c:v>41954.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>41955</c:v>
+                  <c:v>41955.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>41956</c:v>
+                  <c:v>41956.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>41957</c:v>
+                  <c:v>41957.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>41958</c:v>
+                  <c:v>41958.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>41959</c:v>
+                  <c:v>41959.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>41960</c:v>
+                  <c:v>41960.0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>41961</c:v>
+                  <c:v>41961.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -926,97 +931,97 @@
             <c:numRef>
               <c:f>calcs!$E$31:$AH$31</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>41932</c:v>
+                  <c:v>41932.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41933</c:v>
+                  <c:v>41933.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41934</c:v>
+                  <c:v>41934.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41935</c:v>
+                  <c:v>41935.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41936</c:v>
+                  <c:v>41936.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>41937</c:v>
+                  <c:v>41937.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>41938</c:v>
+                  <c:v>41938.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>41939</c:v>
+                  <c:v>41939.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>41940</c:v>
+                  <c:v>41940.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>41941</c:v>
+                  <c:v>41941.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>41942</c:v>
+                  <c:v>41942.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>41943</c:v>
+                  <c:v>41943.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>41944</c:v>
+                  <c:v>41944.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>41945</c:v>
+                  <c:v>41945.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>41946</c:v>
+                  <c:v>41946.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>41947</c:v>
+                  <c:v>41947.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>41948</c:v>
+                  <c:v>41948.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>41949</c:v>
+                  <c:v>41949.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>41950</c:v>
+                  <c:v>41950.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>41951</c:v>
+                  <c:v>41951.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>41952</c:v>
+                  <c:v>41952.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>41953</c:v>
+                  <c:v>41953.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>41954</c:v>
+                  <c:v>41954.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>41955</c:v>
+                  <c:v>41955.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>41956</c:v>
+                  <c:v>41956.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>41957</c:v>
+                  <c:v>41957.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>41958</c:v>
+                  <c:v>41958.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>41959</c:v>
+                  <c:v>41959.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>41960</c:v>
+                  <c:v>41960.0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>41961</c:v>
+                  <c:v>41961.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1317,97 +1322,97 @@
             <c:numRef>
               <c:f>calcs!$E$31:$AH$31</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>41932</c:v>
+                  <c:v>41932.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41933</c:v>
+                  <c:v>41933.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41934</c:v>
+                  <c:v>41934.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41935</c:v>
+                  <c:v>41935.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41936</c:v>
+                  <c:v>41936.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>41937</c:v>
+                  <c:v>41937.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>41938</c:v>
+                  <c:v>41938.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>41939</c:v>
+                  <c:v>41939.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>41940</c:v>
+                  <c:v>41940.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>41941</c:v>
+                  <c:v>41941.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>41942</c:v>
+                  <c:v>41942.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>41943</c:v>
+                  <c:v>41943.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>41944</c:v>
+                  <c:v>41944.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>41945</c:v>
+                  <c:v>41945.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>41946</c:v>
+                  <c:v>41946.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>41947</c:v>
+                  <c:v>41947.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>41948</c:v>
+                  <c:v>41948.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>41949</c:v>
+                  <c:v>41949.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>41950</c:v>
+                  <c:v>41950.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>41951</c:v>
+                  <c:v>41951.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>41952</c:v>
+                  <c:v>41952.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>41953</c:v>
+                  <c:v>41953.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>41954</c:v>
+                  <c:v>41954.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>41955</c:v>
+                  <c:v>41955.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>41956</c:v>
+                  <c:v>41956.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>41957</c:v>
+                  <c:v>41957.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>41958</c:v>
+                  <c:v>41958.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>41959</c:v>
+                  <c:v>41959.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>41960</c:v>
+                  <c:v>41960.0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>41961</c:v>
+                  <c:v>41961.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1419,10 +1424,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>9.3000000000000007</c:v>
+                  <c:v>9.3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.3000000000000007</c:v>
+                  <c:v>9.3</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>#N/A</c:v>
@@ -1577,7 +1582,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.3000000000000007</c:v>
+                  <c:v>9.3</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>#N/A</c:v>
@@ -1711,97 +1716,97 @@
             <c:numRef>
               <c:f>calcs!$E$31:$AH$31</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>41932</c:v>
+                  <c:v>41932.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41933</c:v>
+                  <c:v>41933.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41934</c:v>
+                  <c:v>41934.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41935</c:v>
+                  <c:v>41935.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41936</c:v>
+                  <c:v>41936.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>41937</c:v>
+                  <c:v>41937.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>41938</c:v>
+                  <c:v>41938.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>41939</c:v>
+                  <c:v>41939.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>41940</c:v>
+                  <c:v>41940.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>41941</c:v>
+                  <c:v>41941.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>41942</c:v>
+                  <c:v>41942.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>41943</c:v>
+                  <c:v>41943.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>41944</c:v>
+                  <c:v>41944.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>41945</c:v>
+                  <c:v>41945.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>41946</c:v>
+                  <c:v>41946.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>41947</c:v>
+                  <c:v>41947.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>41948</c:v>
+                  <c:v>41948.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>41949</c:v>
+                  <c:v>41949.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>41950</c:v>
+                  <c:v>41950.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>41951</c:v>
+                  <c:v>41951.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>41952</c:v>
+                  <c:v>41952.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>41953</c:v>
+                  <c:v>41953.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>41954</c:v>
+                  <c:v>41954.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>41955</c:v>
+                  <c:v>41955.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>41956</c:v>
+                  <c:v>41956.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>41957</c:v>
+                  <c:v>41957.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>41958</c:v>
+                  <c:v>41958.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>41959</c:v>
+                  <c:v>41959.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>41960</c:v>
+                  <c:v>41960.0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>41961</c:v>
+                  <c:v>41961.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1813,19 +1818,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>8.3000000000000007</c:v>
+                  <c:v>8.3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.3000000000000007</c:v>
+                  <c:v>8.3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.3000000000000007</c:v>
+                  <c:v>8.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.3000000000000007</c:v>
+                  <c:v>8.3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.3000000000000007</c:v>
+                  <c:v>8.3</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>#N/A</c:v>
@@ -1977,7 +1982,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.3000000000000007</c:v>
+                  <c:v>8.3</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>#N/A</c:v>
@@ -2102,97 +2107,97 @@
             <c:numRef>
               <c:f>calcs!$E$31:$AH$31</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>41932</c:v>
+                  <c:v>41932.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41933</c:v>
+                  <c:v>41933.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41934</c:v>
+                  <c:v>41934.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41935</c:v>
+                  <c:v>41935.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>41936</c:v>
+                  <c:v>41936.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>41937</c:v>
+                  <c:v>41937.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>41938</c:v>
+                  <c:v>41938.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>41939</c:v>
+                  <c:v>41939.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>41940</c:v>
+                  <c:v>41940.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>41941</c:v>
+                  <c:v>41941.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>41942</c:v>
+                  <c:v>41942.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>41943</c:v>
+                  <c:v>41943.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>41944</c:v>
+                  <c:v>41944.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>41945</c:v>
+                  <c:v>41945.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>41946</c:v>
+                  <c:v>41946.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>41947</c:v>
+                  <c:v>41947.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>41948</c:v>
+                  <c:v>41948.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>41949</c:v>
+                  <c:v>41949.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>41950</c:v>
+                  <c:v>41950.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>41951</c:v>
+                  <c:v>41951.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>41952</c:v>
+                  <c:v>41952.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>41953</c:v>
+                  <c:v>41953.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>41954</c:v>
+                  <c:v>41954.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>41955</c:v>
+                  <c:v>41955.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>41956</c:v>
+                  <c:v>41956.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>41957</c:v>
+                  <c:v>41957.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>41958</c:v>
+                  <c:v>41958.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>41959</c:v>
+                  <c:v>41959.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>41960</c:v>
+                  <c:v>41960.0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>41961</c:v>
+                  <c:v>41961.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2204,22 +2209,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>7.3000000000000007</c:v>
+                  <c:v>7.300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.3000000000000007</c:v>
+                  <c:v>7.300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.3000000000000007</c:v>
+                  <c:v>7.300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.3000000000000007</c:v>
+                  <c:v>7.300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.3000000000000007</c:v>
+                  <c:v>7.300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.3000000000000007</c:v>
+                  <c:v>7.300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>#N/A</c:v>
@@ -2371,7 +2376,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.3000000000000007</c:v>
+                  <c:v>7.300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>#N/A</c:v>
@@ -2517,22 +2522,22 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.3000000000000007</c:v>
+                  <c:v>6.300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.3000000000000007</c:v>
+                  <c:v>6.300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.3000000000000007</c:v>
+                  <c:v>6.300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6.3000000000000007</c:v>
+                  <c:v>6.300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.3000000000000007</c:v>
+                  <c:v>6.300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.3000000000000007</c:v>
+                  <c:v>6.300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>#N/A</c:v>
@@ -2684,7 +2689,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.3000000000000007</c:v>
+                  <c:v>6.300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>#N/A</c:v>
@@ -2809,16 +2814,16 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.3000000000000007</c:v>
+                  <c:v>5.300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.3000000000000007</c:v>
+                  <c:v>5.300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.3000000000000007</c:v>
+                  <c:v>5.300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.3000000000000007</c:v>
+                  <c:v>5.300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>#N/A</c:v>
@@ -2970,7 +2975,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.3000000000000007</c:v>
+                  <c:v>5.300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>#N/A</c:v>
@@ -3113,31 +3118,31 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.3000000000000007</c:v>
+                  <c:v>4.300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.3000000000000007</c:v>
+                  <c:v>4.300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.3000000000000007</c:v>
+                  <c:v>4.300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4.3000000000000007</c:v>
+                  <c:v>4.300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.3000000000000007</c:v>
+                  <c:v>4.300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4.3000000000000007</c:v>
+                  <c:v>4.300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4.3000000000000007</c:v>
+                  <c:v>4.300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4.3000000000000007</c:v>
+                  <c:v>4.300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.3000000000000007</c:v>
+                  <c:v>4.300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>#N/A</c:v>
@@ -3292,7 +3297,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.3000000000000007</c:v>
+                  <c:v>4.300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>#N/A</c:v>
@@ -3417,22 +3422,22 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.3000000000000007</c:v>
+                  <c:v>3.300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.3000000000000007</c:v>
+                  <c:v>3.300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.3000000000000007</c:v>
+                  <c:v>3.300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.3000000000000007</c:v>
+                  <c:v>3.300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.3000000000000007</c:v>
+                  <c:v>3.300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.3000000000000007</c:v>
+                  <c:v>3.300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>#N/A</c:v>
@@ -3584,7 +3589,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.3000000000000007</c:v>
+                  <c:v>3.300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>#N/A</c:v>
@@ -3635,7 +3640,7 @@
             <c:errBarType val="both"/>
             <c:errValType val="fixedVal"/>
             <c:noEndCap val="0"/>
-            <c:val val="10"/>
+            <c:val val="10.0"/>
             <c:spPr>
               <a:ln w="263525">
                 <a:solidFill>
@@ -3656,7 +3661,7 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>#N/A</c:v>
@@ -6926,94 +6931,94 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>2.3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>2.3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>2.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>2.3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>2.3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>2.3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>2.3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>2.3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>2.3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>2.3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>2.3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>2.3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>2.3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>2.3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>2.3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>2.3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>2.3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>2.3</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>2.3</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>2.3</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>2.3</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>2.3</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>2.3</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>2.3</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>2.3</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>2.3</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>2.3</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>2.3</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>2.3</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>2.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7051,40 +7056,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>13</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>13</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>13</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>13</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>13</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>13</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>13</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>#N/A</c:v>
@@ -7212,58 +7217,58 @@
                   <c:v>#N/A</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>13</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>13</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>13</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>13</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>13</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>13</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>13</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>13</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>13</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>13</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>13</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>13</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>13</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>13</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>13</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>13</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7280,11 +7285,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="695353440"/>
-        <c:axId val="695354000"/>
+        <c:axId val="2080498920"/>
+        <c:axId val="2037870824"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="695353440"/>
+        <c:axId val="2080498920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7307,18 +7312,18 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="695354000"/>
+        <c:crossAx val="2037870824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="695354000"/>
+        <c:axId val="2037870824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="13.5"/>
-          <c:min val="0"/>
+          <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="l"/>
@@ -7326,10 +7331,10 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="695353440"/>
+        <c:crossAx val="2080498920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="1"/>
+        <c:majorUnit val="1.0"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
@@ -7354,7 +7359,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="1" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="1.0" header="0.3" footer="0.3"/>
     <c:pageSetup orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -7401,19 +7406,19 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>47625</xdr:colOff>
+          <xdr:colOff>50800</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>209549</xdr:rowOff>
+          <xdr:rowOff>215900</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>6</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>17</xdr:row>
-          <xdr:rowOff>28574</xdr:rowOff>
+          <xdr:rowOff>25400</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1025" name="Scroll Bar" descr="Click the scroll bar to modify the project time frame shown on the Timeline Chart or enter the start date for the display of project activities in cell D20." hidden="1">
+            <xdr:cNvPr id="1025" name="Scroll Bar" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1025"/>
@@ -7422,7 +7427,7 @@
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -7430,12 +7435,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="9525">
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
@@ -7701,28 +7700,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1">
+  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0">
     <tabColor theme="5"/>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="5.5" style="8" customWidth="1"/>
     <col min="2" max="2" width="0" style="8" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="34.5703125" style="8" customWidth="1"/>
-    <col min="4" max="5" width="18.42578125" style="8" customWidth="1"/>
-    <col min="6" max="6" width="100.85546875" style="8" customWidth="1"/>
-    <col min="7" max="7" width="5.5703125" style="8" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="8"/>
+    <col min="3" max="3" width="34.5" style="8" customWidth="1"/>
+    <col min="4" max="5" width="18.5" style="8" customWidth="1"/>
+    <col min="6" max="6" width="100.83203125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="5.5" style="8" customWidth="1"/>
+    <col min="8" max="16384" width="8.83203125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="7" customFormat="1" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="7" customFormat="1" ht="47.25" customHeight="1" thickBot="1">
       <c r="A1" s="4"/>
       <c r="B1" s="5"/>
       <c r="C1" s="19" t="s">
@@ -7733,22 +7732,22 @@
       <c r="F1" s="4"/>
       <c r="G1" s="6"/>
     </row>
-    <row r="2" spans="1:7" ht="17.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="17.25" customHeight="1" thickTop="1">
       <c r="C2" s="9"/>
     </row>
-    <row r="15" spans="1:7" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="17.25" customHeight="1" thickBot="1">
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
     </row>
-    <row r="16" spans="1:7" ht="17.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="17.25" customHeight="1" thickTop="1">
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
     </row>
-    <row r="17" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" ht="17.25" customHeight="1">
       <c r="C17" s="17" t="s">
         <v>19</v>
       </c>
@@ -7758,13 +7757,13 @@
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
     </row>
-    <row r="18" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:6" ht="17.25" customHeight="1">
       <c r="C18" s="11"/>
       <c r="D18" s="11"/>
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
     </row>
-    <row r="19" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:6" ht="17.25" customHeight="1">
       <c r="B19" s="12" t="s">
         <v>5</v>
       </c>
@@ -7781,7 +7780,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:6" ht="17.25" customHeight="1">
       <c r="B20" s="12">
         <f t="shared" ref="B20:B25" si="0">N(B19)+1</f>
         <v>1</v>
@@ -7795,7 +7794,7 @@
       <c r="E20" s="15"/>
       <c r="F20" s="14"/>
     </row>
-    <row r="21" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:6" ht="17.25" customHeight="1">
       <c r="B21" s="12">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -7809,7 +7808,7 @@
       <c r="E21" s="15"/>
       <c r="F21" s="20"/>
     </row>
-    <row r="22" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:6" ht="17.25" customHeight="1">
       <c r="B22" s="12">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -7819,7 +7818,7 @@
       <c r="E22" s="15"/>
       <c r="F22" s="14"/>
     </row>
-    <row r="23" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:6" ht="17.25" customHeight="1">
       <c r="B23" s="12">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -7833,7 +7832,7 @@
       <c r="E23" s="15"/>
       <c r="F23" s="14"/>
     </row>
-    <row r="24" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:6" ht="17.25" customHeight="1">
       <c r="B24" s="12">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -7847,7 +7846,7 @@
       <c r="E24" s="15"/>
       <c r="F24" s="14"/>
     </row>
-    <row r="25" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:6" ht="17.25" customHeight="1">
       <c r="B25" s="12">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -7861,7 +7860,7 @@
       <c r="E25" s="15"/>
       <c r="F25" s="14"/>
     </row>
-    <row r="26" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:6" ht="17.25" customHeight="1">
       <c r="B26" s="16">
         <f t="shared" ref="B26:B31" si="1">N(B25)+1</f>
         <v>7</v>
@@ -7875,7 +7874,7 @@
       <c r="E26" s="15"/>
       <c r="F26" s="14"/>
     </row>
-    <row r="27" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:6" ht="17.25" customHeight="1">
       <c r="B27" s="16">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -7885,7 +7884,7 @@
       <c r="E27" s="15"/>
       <c r="F27" s="14"/>
     </row>
-    <row r="28" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:6" ht="17.25" customHeight="1">
       <c r="B28" s="16">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -7903,7 +7902,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:6" ht="17.25" customHeight="1">
       <c r="B29" s="16">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -7921,7 +7920,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:6" ht="17.25" customHeight="1">
       <c r="B30" s="16">
         <f>N(B29)+1</f>
         <v>11</v>
@@ -7939,7 +7938,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:6" ht="17.25" customHeight="1">
       <c r="B31" s="16">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -7949,7 +7948,7 @@
       <c r="E31" s="22"/>
       <c r="F31" s="14"/>
     </row>
-    <row r="32" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:6" ht="17.25" customHeight="1">
       <c r="B32" s="8">
         <f>N(B31)+1</f>
         <v>13</v>
@@ -7967,7 +7966,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:6" ht="17.25" customHeight="1">
       <c r="B33" s="8">
         <f>N(B32)+1</f>
         <v>14</v>
@@ -7985,7 +7984,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:6" ht="17.25" customHeight="1">
       <c r="B34" s="8">
         <f t="shared" ref="B34:B44" si="2">N(B33)+1</f>
         <v>15</v>
@@ -7995,7 +7994,7 @@
       <c r="E34" s="22"/>
       <c r="F34" s="21"/>
     </row>
-    <row r="35" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:6" ht="17.25" customHeight="1">
       <c r="B35" s="8">
         <f t="shared" si="2"/>
         <v>16</v>
@@ -8013,7 +8012,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:6" ht="17.25" customHeight="1">
       <c r="B36" s="8">
         <f t="shared" si="2"/>
         <v>17</v>
@@ -8031,7 +8030,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:6" ht="17.25" customHeight="1">
       <c r="B37" s="8">
         <f t="shared" si="2"/>
         <v>18</v>
@@ -8041,7 +8040,7 @@
       <c r="E37" s="22"/>
       <c r="F37" s="21"/>
     </row>
-    <row r="38" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:6" ht="17.25" customHeight="1">
       <c r="B38" s="8">
         <f>N(B37)+1</f>
         <v>19</v>
@@ -8059,7 +8058,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:6" ht="17.25" customHeight="1">
       <c r="B39" s="8">
         <f>N(B38)+1</f>
         <v>20</v>
@@ -8077,7 +8076,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:6" ht="17.25" customHeight="1">
       <c r="B40" s="8">
         <f t="shared" si="2"/>
         <v>21</v>
@@ -8087,7 +8086,7 @@
       <c r="E40" s="22"/>
       <c r="F40" s="21"/>
     </row>
-    <row r="41" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:6" ht="17.25" customHeight="1">
       <c r="B41" s="8">
         <f t="shared" si="2"/>
         <v>22</v>
@@ -8105,7 +8104,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="42" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:6" ht="17.25" customHeight="1">
       <c r="B42" s="8">
         <f t="shared" si="2"/>
         <v>23</v>
@@ -8123,7 +8122,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:6" ht="17.25" customHeight="1">
       <c r="B43" s="8">
         <f t="shared" si="2"/>
         <v>24</v>
@@ -8133,7 +8132,7 @@
       <c r="E43" s="22"/>
       <c r="F43" s="21"/>
     </row>
-    <row r="44" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:6" ht="17.25" customHeight="1">
       <c r="B44" s="8">
         <f t="shared" si="2"/>
         <v>25</v>
@@ -8151,7 +8150,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:6" ht="17.25" customHeight="1">
       <c r="B45" s="8">
         <f t="shared" ref="B45:B61" si="3">N(B44)+1</f>
         <v>26</v>
@@ -8169,7 +8168,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:6" ht="17.25" customHeight="1">
       <c r="B46" s="8">
         <f t="shared" si="3"/>
         <v>27</v>
@@ -8179,7 +8178,7 @@
       <c r="E46" s="22"/>
       <c r="F46" s="21"/>
     </row>
-    <row r="47" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:6" ht="17.25" customHeight="1">
       <c r="B47" s="8">
         <f t="shared" si="3"/>
         <v>28</v>
@@ -8197,7 +8196,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="48" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:6" ht="17.25" customHeight="1">
       <c r="B48" s="8">
         <f t="shared" si="3"/>
         <v>29</v>
@@ -8207,7 +8206,7 @@
       <c r="E48" s="22"/>
       <c r="F48" s="21"/>
     </row>
-    <row r="49" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:6" ht="17.25" customHeight="1">
       <c r="B49" s="8">
         <f t="shared" si="3"/>
         <v>30</v>
@@ -8225,7 +8224,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="50" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:6" ht="17.25" customHeight="1">
       <c r="B50" s="8">
         <f t="shared" si="3"/>
         <v>31</v>
@@ -8243,7 +8242,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="51" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:6" ht="17.25" customHeight="1">
       <c r="B51" s="8">
         <f t="shared" si="3"/>
         <v>32</v>
@@ -8253,7 +8252,7 @@
       <c r="E51" s="22"/>
       <c r="F51" s="21"/>
     </row>
-    <row r="52" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:6" ht="17.25" customHeight="1">
       <c r="B52" s="8">
         <f t="shared" si="3"/>
         <v>33</v>
@@ -8263,7 +8262,7 @@
       <c r="E52" s="22"/>
       <c r="F52" s="21"/>
     </row>
-    <row r="53" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:6" ht="17.25" customHeight="1">
       <c r="B53" s="8">
         <f t="shared" si="3"/>
         <v>34</v>
@@ -8273,7 +8272,7 @@
       <c r="E53" s="22"/>
       <c r="F53" s="21"/>
     </row>
-    <row r="54" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:6" ht="17.25" customHeight="1">
       <c r="B54" s="8">
         <f t="shared" si="3"/>
         <v>35</v>
@@ -8283,7 +8282,7 @@
       <c r="E54" s="22"/>
       <c r="F54" s="21"/>
     </row>
-    <row r="55" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:6" ht="17.25" customHeight="1">
       <c r="B55" s="8">
         <f t="shared" si="3"/>
         <v>36</v>
@@ -8293,7 +8292,7 @@
       <c r="E55" s="22"/>
       <c r="F55" s="21"/>
     </row>
-    <row r="56" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:6" ht="17.25" customHeight="1">
       <c r="B56" s="8">
         <f t="shared" si="3"/>
         <v>37</v>
@@ -8303,7 +8302,7 @@
       <c r="E56" s="22"/>
       <c r="F56" s="21"/>
     </row>
-    <row r="57" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:6" ht="17.25" customHeight="1">
       <c r="B57" s="8">
         <f t="shared" si="3"/>
         <v>38</v>
@@ -8313,7 +8312,7 @@
       <c r="E57" s="22"/>
       <c r="F57" s="21"/>
     </row>
-    <row r="58" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:6" ht="17.25" customHeight="1">
       <c r="B58" s="8">
         <f t="shared" si="3"/>
         <v>39</v>
@@ -8323,7 +8322,7 @@
       <c r="E58" s="22"/>
       <c r="F58" s="21"/>
     </row>
-    <row r="59" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:6" ht="17.25" customHeight="1">
       <c r="B59" s="8">
         <f t="shared" si="3"/>
         <v>40</v>
@@ -8333,7 +8332,7 @@
       <c r="E59" s="22"/>
       <c r="F59" s="21"/>
     </row>
-    <row r="60" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:6" ht="17.25" customHeight="1">
       <c r="B60" s="8">
         <f t="shared" si="3"/>
         <v>41</v>
@@ -8343,7 +8342,7 @@
       <c r="E60" s="22"/>
       <c r="F60" s="21"/>
     </row>
-    <row r="61" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:6" ht="17.25" customHeight="1">
       <c r="B61" s="8">
         <f t="shared" si="3"/>
         <v>42</v>
@@ -8357,70 +8356,76 @@
   <sheetProtection selectLockedCells="1"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <rowBreaks count="2" manualBreakCount="2">
     <brk id="15" max="16383" man="1"/>
     <brk id="17" max="16383" man="1"/>
   </rowBreaks>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x14">
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1025" r:id="rId4" name="Scroll Bar">
+            <control shapeId="1025" r:id="rId3" name="Scroll Bar">
               <controlPr defaultSize="0" autoPict="0" altText="Click the scroll bar to modify the project time frame shown on the Timeline Chart or enter the start date for the display of project activities in cell D20.">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>4</xdr:col>
-                    <xdr:colOff>47625</xdr:colOff>
+                    <xdr:colOff>50800</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>209550</xdr:rowOff>
+                    <xdr:rowOff>215900</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>6</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
                     <xdr:row>17</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
+                    <xdr:rowOff>25400</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
       </controls>
     </mc:Choice>
+    <mc:Fallback/>
   </mc:AlternateContent>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet2"/>
+  <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AI72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.5" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="34" width="10.85546875" customWidth="1"/>
-    <col min="35" max="35" width="17.5703125" customWidth="1"/>
+    <col min="5" max="34" width="10.83203125" customWidth="1"/>
+    <col min="35" max="35" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="C3" t="s">
         <v>10</v>
       </c>
@@ -8430,30 +8435,30 @@
       </c>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="D4">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="E6" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="E7" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="E8" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="C9" s="2" t="s">
         <v>12</v>
       </c>
@@ -8466,7 +8471,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="D10">
         <v>9</v>
       </c>
@@ -8475,7 +8480,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="D11">
         <f>D10-MIN(D10,D9)</f>
         <v>0</v>
@@ -8485,27 +8490,27 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="E12" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="C13" s="2"/>
       <c r="E13" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="C14" s="2"/>
       <c r="E14" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="C15" s="2"/>
       <c r="E15">
         <f t="array" ref="E15">INDEX(Activities[Id],MATCH(1, ((Activities[START]&gt;=StartDateWindow)+(Activities[END]&gt;=StartDateWindow)&gt;0)*(Activities[START]&lt;=(StartDateWindow+WindowDays-1)), 0))</f>
@@ -8516,7 +8521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="C16" s="2"/>
       <c r="E16">
         <f t="array" ref="E16">INDEX(Activities[Id],MATCH(1, (Activities[Id]&gt;E15)*((Activities[START]&gt;=StartDateWindow)+(Activities[END]&gt;=StartDateWindow)&gt;0)*(Activities[START]&lt;=(StartDateWindow+WindowDays-1)), 0))</f>
@@ -8527,7 +8532,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:35">
       <c r="C17" s="2"/>
       <c r="E17">
         <f t="array" ref="E17">INDEX(Activities[Id],MATCH(1, (Activities[Id]&gt;E16)*((Activities[START]&gt;=StartDateWindow)+(Activities[END]&gt;=StartDateWindow)&gt;0)*(Activities[START]&lt;=(StartDateWindow+WindowDays-1)), 0))</f>
@@ -8538,7 +8543,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:35">
       <c r="E18">
         <f t="array" ref="E18">INDEX(Activities[Id],MATCH(1, (Activities[Id]&gt;E17)*((Activities[START]&gt;=StartDateWindow)+(Activities[END]&gt;=StartDateWindow)&gt;0)*(Activities[START]&lt;=(StartDateWindow+WindowDays-1)), 0))</f>
         <v>10</v>
@@ -8548,7 +8553,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:35">
       <c r="E19">
         <f t="array" ref="E19">INDEX(Activities[Id],MATCH(1, (Activities[Id]&gt;E18)*((Activities[START]&gt;=StartDateWindow)+(Activities[END]&gt;=StartDateWindow)&gt;0)*(Activities[START]&lt;=(StartDateWindow+WindowDays-1)), 0))</f>
         <v>11</v>
@@ -8558,7 +8563,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:35">
       <c r="E20">
         <f t="array" ref="E20">INDEX(Activities[Id],MATCH(1, (Activities[Id]&gt;E19)*((Activities[START]&gt;=StartDateWindow)+(Activities[END]&gt;=StartDateWindow)&gt;0)*(Activities[START]&lt;=(StartDateWindow+WindowDays-1)), 0))</f>
         <v>13</v>
@@ -8568,7 +8573,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:35">
       <c r="E21">
         <f t="array" ref="E21">INDEX(Activities[Id],MATCH(1, (Activities[Id]&gt;E20)*((Activities[START]&gt;=StartDateWindow)+(Activities[END]&gt;=StartDateWindow)&gt;0)*(Activities[START]&lt;=(StartDateWindow+WindowDays-1)), 0))</f>
         <v>14</v>
@@ -8578,7 +8583,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:35">
       <c r="E22">
         <f t="array" ref="E22">INDEX(Activities[Id],MATCH(1, (Activities[Id]&gt;E21)*((Activities[START]&gt;=StartDateWindow)+(Activities[END]&gt;=StartDateWindow)&gt;0)*(Activities[START]&lt;=(StartDateWindow+WindowDays-1)), 0))</f>
         <v>16</v>
@@ -8588,7 +8593,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:35">
       <c r="E23">
         <f t="array" ref="E23">INDEX(Activities[Id],MATCH(1, (Activities[Id]&gt;E22)*((Activities[START]&gt;=StartDateWindow)+(Activities[END]&gt;=StartDateWindow)&gt;0)*(Activities[START]&lt;=(StartDateWindow+WindowDays-1)), 0))</f>
         <v>17</v>
@@ -8598,7 +8603,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:35">
       <c r="C25" t="s">
         <v>4</v>
       </c>
@@ -8607,7 +8612,7 @@
         <v>41932</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:35">
       <c r="C26" t="s">
         <v>3</v>
       </c>
@@ -8615,7 +8620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:35">
       <c r="C28" t="s">
         <v>1</v>
       </c>
@@ -8624,7 +8629,7 @@
         <v>41932</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:35">
       <c r="C29" t="s">
         <v>2</v>
       </c>
@@ -8632,7 +8637,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:35">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -8770,7 +8775,7 @@
         <v>41962</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:35">
       <c r="A32">
         <v>11.3</v>
       </c>
@@ -8910,7 +8915,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:35">
       <c r="A33">
         <f>A32-1</f>
         <v>10.3</v>
@@ -9051,7 +9056,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:35">
       <c r="A34">
         <f t="shared" ref="A34:A40" si="3">A33-1</f>
         <v>9.3000000000000007</v>
@@ -9192,7 +9197,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:35">
       <c r="A35">
         <f t="shared" si="3"/>
         <v>8.3000000000000007</v>
@@ -9333,7 +9338,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:35">
       <c r="A36">
         <f t="shared" si="3"/>
         <v>7.3000000000000007</v>
@@ -9474,7 +9479,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:35">
       <c r="A37">
         <f t="shared" si="3"/>
         <v>6.3000000000000007</v>
@@ -9615,7 +9620,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:35">
       <c r="A38">
         <f t="shared" si="3"/>
         <v>5.3000000000000007</v>
@@ -9756,7 +9761,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:35">
       <c r="A39">
         <f t="shared" si="3"/>
         <v>4.3000000000000007</v>
@@ -9897,7 +9902,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:35">
       <c r="A40">
         <f t="shared" si="3"/>
         <v>3.3000000000000007</v>
@@ -10038,7 +10043,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="43" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:35">
       <c r="E43" s="1">
         <f>E31</f>
         <v>41932</v>
@@ -10160,7 +10165,7 @@
         <v>41961</v>
       </c>
     </row>
-    <row r="44" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:35">
       <c r="C44">
         <f ca="1">C32</f>
         <v>1</v>
@@ -10290,7 +10295,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="45" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:35">
       <c r="C45">
         <f t="shared" ref="C45:C52" ca="1" si="6">C33</f>
         <v>4</v>
@@ -10420,7 +10425,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="46" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:35">
       <c r="C46">
         <f t="shared" ca="1" si="6"/>
         <v>9</v>
@@ -10550,7 +10555,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="47" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:35">
       <c r="C47">
         <f t="shared" ca="1" si="6"/>
         <v>10</v>
@@ -10680,7 +10685,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="48" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:35">
       <c r="C48">
         <f t="shared" ca="1" si="6"/>
         <v>11</v>
@@ -10810,7 +10815,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="49" spans="3:34" x14ac:dyDescent="0.2">
+    <row r="49" spans="3:34">
       <c r="C49">
         <f t="shared" ca="1" si="6"/>
         <v>13</v>
@@ -10940,7 +10945,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="50" spans="3:34" x14ac:dyDescent="0.2">
+    <row r="50" spans="3:34">
       <c r="C50">
         <f t="shared" ca="1" si="6"/>
         <v>14</v>
@@ -11070,7 +11075,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="51" spans="3:34" x14ac:dyDescent="0.2">
+    <row r="51" spans="3:34">
       <c r="C51">
         <f t="shared" ca="1" si="6"/>
         <v>16</v>
@@ -11200,7 +11205,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="52" spans="3:34" x14ac:dyDescent="0.2">
+    <row r="52" spans="3:34">
       <c r="C52">
         <f t="shared" ca="1" si="6"/>
         <v>17</v>
@@ -11330,7 +11335,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="55" spans="3:34" x14ac:dyDescent="0.2">
+    <row r="55" spans="3:34">
       <c r="E55" s="1">
         <f>E31</f>
         <v>41932</v>
@@ -11452,7 +11457,7 @@
         <v>41961</v>
       </c>
     </row>
-    <row r="56" spans="3:34" x14ac:dyDescent="0.2">
+    <row r="56" spans="3:34">
       <c r="D56" t="s">
         <v>11</v>
       </c>
@@ -11577,7 +11582,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="58" spans="3:34" x14ac:dyDescent="0.2">
+    <row r="58" spans="3:34">
       <c r="D58" s="3">
         <f>DATE(YEAR(MIN(E55:AH55)),MONTH(MIN(E55:AH55)),1)</f>
         <v>41913</v>
@@ -11703,7 +11708,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="59" spans="3:34" x14ac:dyDescent="0.2">
+    <row r="59" spans="3:34">
       <c r="D59" s="3" t="str">
         <f>TEXT(D58,"mmm yyyy") &amp; " - Top Band"</f>
         <v>Oct 2014 - Top Band</v>
@@ -11829,10 +11834,10 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="60" spans="3:34" x14ac:dyDescent="0.2">
+    <row r="60" spans="3:34">
       <c r="D60" s="3"/>
     </row>
-    <row r="61" spans="3:34" x14ac:dyDescent="0.2">
+    <row r="61" spans="3:34">
       <c r="D61" s="3">
         <f>EOMONTH(D58,0)+1</f>
         <v>41944</v>
@@ -11958,7 +11963,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="62" spans="3:34" x14ac:dyDescent="0.2">
+    <row r="62" spans="3:34">
       <c r="D62" s="3" t="str">
         <f>TEXT(D61,"mmm yyyy") &amp; " - Top Band"</f>
         <v>Nov 2014 - Top Band</v>
@@ -12084,10 +12089,10 @@
         <v>13</v>
       </c>
     </row>
-    <row r="63" spans="3:34" x14ac:dyDescent="0.2">
+    <row r="63" spans="3:34">
       <c r="D63" s="3"/>
     </row>
-    <row r="65" spans="4:34" x14ac:dyDescent="0.2">
+    <row r="65" spans="4:34">
       <c r="D65" s="3">
         <f>D58+1</f>
         <v>41914</v>
@@ -12213,7 +12218,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="66" spans="4:34" x14ac:dyDescent="0.2">
+    <row r="66" spans="4:34">
       <c r="D66" s="3">
         <f>D61+1</f>
         <v>41945</v>
@@ -12339,7 +12344,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="69" spans="4:34" x14ac:dyDescent="0.2">
+    <row r="69" spans="4:34">
       <c r="E69">
         <v>2.2999999999999998</v>
       </c>
@@ -12460,7 +12465,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="70" spans="4:34" x14ac:dyDescent="0.2">
+    <row r="70" spans="4:34">
       <c r="D70">
         <v>3</v>
       </c>
@@ -12585,7 +12590,7 @@
         <v>TUE</v>
       </c>
     </row>
-    <row r="71" spans="4:34" x14ac:dyDescent="0.2">
+    <row r="71" spans="4:34">
       <c r="E71">
         <v>1.3</v>
       </c>
@@ -12706,7 +12711,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="72" spans="4:34" x14ac:dyDescent="0.2">
+    <row r="72" spans="4:34">
       <c r="E72" t="str">
         <f>TEXT(E55,"dd")</f>
         <v>20</v>
@@ -12830,23 +12835,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>AssetEditForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2CD552CE-B979-4BDB-9FB1-264C1B806DC7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>